<commit_message>
cleaned data and script
</commit_message>
<xml_diff>
--- a/data/metadada.xlsx
+++ b/data/metadada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/M.Sc/forestSlideERRA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BDBF75-086E-1948-B2DE-AB0AB4D6706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B7FD8-8917-0C44-B303-88490B20DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{944107A5-B329-F14B-9A6E-1760380B00FD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{944107A5-B329-F14B-9A6E-1760380B00FD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="hydrometric" sheetId="1" r:id="rId3"/>
     <sheet name="climate" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>River</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>Big Creek</t>
+  </si>
+  <si>
+    <t>Downloaded</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -745,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C35812-5A39-4745-A4EB-7DA0BCEFD1B1}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -907,15 +916,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4CBCD0-3701-AB48-A663-3C82C1076C80}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -934,8 +943,11 @@
       <c r="F1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -954,8 +966,11 @@
       <c r="F2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -973,6 +988,9 @@
       </c>
       <c r="F3" t="s">
         <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardize q by catchment area, now in mm/day
</commit_message>
<xml_diff>
--- a/data/metadada.xlsx
+++ b/data/metadada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/M.Sc/forestSlideERRA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B7FD8-8917-0C44-B303-88490B20DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FC8049-9F13-1943-9B4A-1087B868900F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{944107A5-B329-F14B-9A6E-1760380B00FD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{944107A5-B329-F14B-9A6E-1760380B00FD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Area (Ha)</t>
-  </si>
-  <si>
     <t>Watersheds tab</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Area (m^2)</t>
   </si>
 </sst>
 </file>
@@ -630,18 +630,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -649,7 +649,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C35812-5A39-4745-A4EB-7DA0BCEFD1B1}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,20 +768,20 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
-        <f>C2*0.01</f>
+        <f>C2*10000</f>
         <v>0</v>
       </c>
       <c r="E2" s="1"/>
@@ -790,25 +790,27 @@
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>1567.29</v>
+      </c>
       <c r="D3">
-        <f>C3*0.01</f>
-        <v>0</v>
+        <f>C3*10000</f>
+        <v>15672900</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +823,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -891,7 +893,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>1159</v>
@@ -918,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4CBCD0-3701-AB48-A663-3C82C1076C80}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -944,7 +946,7 @@
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -967,7 +969,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -990,7 +992,7 @@
         <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>